<commit_message>
fixed correalted random effects
</commit_message>
<xml_diff>
--- a/Output/00_PrettyEditedTables.xlsx
+++ b/Output/00_PrettyEditedTables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kueng\DataAnalysis\02TimeAndTiesControl_updatedBRMS\Output\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pascku\Repos\02TimeAndTiesControl\Output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C016BF9B-0F7F-4D04-88C7-B0B951BFB19A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5079B08F-ACC9-409D-ACA2-36935569E4D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19303" yWindow="3369" windowWidth="19406" windowHeight="11485" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MVPA" sheetId="2" r:id="rId1"/>
@@ -770,7 +770,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -817,6 +817,13 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -898,7 +905,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -945,18 +952,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -971,6 +966,21 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1270,63 +1280,63 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E876E58-69A6-40D5-A138-00AF2B8A39AF}">
   <dimension ref="A2:I36"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" zoomScale="94" workbookViewId="0">
-      <selection activeCell="L28" sqref="L28"/>
+    <sheetView tabSelected="1" zoomScale="94" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="43.36328125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.453125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="15.40625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="43.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.46484375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="15.3984375" style="3" customWidth="1"/>
     <col min="4" max="4" width="0.86328125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="11.453125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="15.40625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="11.46484375" style="3" customWidth="1"/>
+    <col min="6" max="6" width="15.3984375" style="3" customWidth="1"/>
     <col min="7" max="7" width="0.86328125" style="3" customWidth="1"/>
-    <col min="8" max="8" width="11.453125" style="3" customWidth="1"/>
-    <col min="9" max="9" width="15.40625" style="3" customWidth="1"/>
-    <col min="10" max="16384" width="8.7265625" style="3"/>
+    <col min="8" max="8" width="11.46484375" style="3" customWidth="1"/>
+    <col min="9" max="9" width="15.3984375" style="3" customWidth="1"/>
+    <col min="10" max="16384" width="8.73046875" style="3"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A2" s="1"/>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="22" t="s">
         <v>101</v>
       </c>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
       <c r="G2" s="2"/>
-      <c r="H2" s="17" t="s">
+      <c r="H2" s="22" t="s">
         <v>154</v>
       </c>
-      <c r="I2" s="17" t="s">
+      <c r="I2" s="22" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="21" t="s">
         <v>99</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="21" t="s">
         <v>1</v>
       </c>
       <c r="D3" s="4"/>
-      <c r="E3" s="16" t="s">
+      <c r="E3" s="21" t="s">
         <v>100</v>
       </c>
-      <c r="F3" s="16"/>
+      <c r="F3" s="21"/>
       <c r="G3" s="4"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="16" t="s">
+      <c r="H3" s="21"/>
+      <c r="I3" s="21" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" s="15" t="s">
         <v>155</v>
       </c>
@@ -1351,7 +1361,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
@@ -1376,28 +1386,28 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.75">
-      <c r="A6" s="19" t="s">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A6" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="19" t="s">
+      <c r="C6" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="19"/>
-      <c r="H6" s="19" t="s">
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="I6" s="19" t="s">
+      <c r="I6" s="24" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A7" s="8" t="s">
         <v>13</v>
       </c>
@@ -1422,7 +1432,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A8" s="8" t="s">
         <v>102</v>
       </c>
@@ -1447,7 +1457,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A9" s="8" t="s">
         <v>16</v>
       </c>
@@ -1458,7 +1468,7 @@
         <v>115</v>
       </c>
       <c r="D9" s="7"/>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="25" t="s">
         <v>17</v>
       </c>
       <c r="F9" s="7" t="s">
@@ -1472,7 +1482,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A10" s="8" t="s">
         <v>103</v>
       </c>
@@ -1497,7 +1507,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A11" s="8" t="s">
         <v>20</v>
       </c>
@@ -1522,7 +1532,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A12" s="8" t="s">
         <v>104</v>
       </c>
@@ -1547,7 +1557,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A13" s="8" t="s">
         <v>27</v>
       </c>
@@ -1572,7 +1582,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A14" s="8" t="s">
         <v>29</v>
       </c>
@@ -1597,7 +1607,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A15" s="8" t="s">
         <v>32</v>
       </c>
@@ -1622,7 +1632,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A16" s="8" t="s">
         <v>35</v>
       </c>
@@ -1639,28 +1649,28 @@
         <v>135</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.75">
-      <c r="A17" s="19" t="s">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A17" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="B17" s="19" t="s">
+      <c r="B17" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="C17" s="19" t="s">
+      <c r="C17" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="D17" s="19"/>
-      <c r="E17" s="19"/>
-      <c r="F17" s="19"/>
-      <c r="G17" s="19"/>
-      <c r="H17" s="19" t="s">
+      <c r="D17" s="24"/>
+      <c r="E17" s="24"/>
+      <c r="F17" s="24"/>
+      <c r="G17" s="24"/>
+      <c r="H17" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="I17" s="19" t="s">
+      <c r="I17" s="24" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A18" s="8" t="s">
         <v>38</v>
       </c>
@@ -1685,7 +1695,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A19" s="8" t="s">
         <v>105</v>
       </c>
@@ -1710,7 +1720,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A20" s="8" t="s">
         <v>41</v>
       </c>
@@ -1735,7 +1745,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A21" s="8" t="s">
         <v>106</v>
       </c>
@@ -1760,7 +1770,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A22" s="8" t="s">
         <v>43</v>
       </c>
@@ -1785,7 +1795,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A23" s="8" t="s">
         <v>107</v>
       </c>
@@ -1810,7 +1820,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A24" s="8" t="s">
         <v>48</v>
       </c>
@@ -1827,7 +1837,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
       <c r="B25" s="7"/>
       <c r="C25" s="7"/>
       <c r="D25" s="7"/>
@@ -1837,45 +1847,45 @@
       <c r="H25" s="7"/>
       <c r="I25" s="7"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A26" s="1"/>
-      <c r="B26" s="17" t="s">
+      <c r="B26" s="22" t="s">
         <v>101</v>
       </c>
-      <c r="C26" s="17"/>
-      <c r="D26" s="17"/>
-      <c r="E26" s="17"/>
-      <c r="F26" s="17"/>
+      <c r="C26" s="22"/>
+      <c r="D26" s="22"/>
+      <c r="E26" s="22"/>
+      <c r="F26" s="22"/>
       <c r="G26" s="2"/>
-      <c r="H26" s="17" t="s">
+      <c r="H26" s="22" t="s">
         <v>154</v>
       </c>
-      <c r="I26" s="17" t="s">
+      <c r="I26" s="22" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A27" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="18" t="s">
+      <c r="B27" s="23" t="s">
         <v>99</v>
       </c>
-      <c r="C27" s="18" t="s">
+      <c r="C27" s="23" t="s">
         <v>1</v>
       </c>
       <c r="D27" s="10"/>
-      <c r="E27" s="18" t="s">
+      <c r="E27" s="23" t="s">
         <v>100</v>
       </c>
-      <c r="F27" s="18"/>
+      <c r="F27" s="23"/>
       <c r="G27" s="10"/>
-      <c r="H27" s="18"/>
-      <c r="I27" s="18" t="s">
+      <c r="H27" s="23"/>
+      <c r="I27" s="23" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="16.5" x14ac:dyDescent="0.75">
+    <row r="28" spans="1:9" ht="15.75" x14ac:dyDescent="0.45">
       <c r="A28" s="11" t="s">
         <v>60</v>
       </c>
@@ -1900,7 +1910,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A29" s="3" t="s">
         <v>6</v>
       </c>
@@ -1925,7 +1935,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A30" s="3" t="s">
         <v>13</v>
       </c>
@@ -1950,7 +1960,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A31" s="3" t="s">
         <v>102</v>
       </c>
@@ -1975,7 +1985,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A32" s="3" t="s">
         <v>16</v>
       </c>
@@ -2000,7 +2010,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A33" s="3" t="s">
         <v>103</v>
       </c>
@@ -2025,7 +2035,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A34" s="3" t="s">
         <v>20</v>
       </c>
@@ -2050,7 +2060,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A35" s="3" t="s">
         <v>104</v>
       </c>
@@ -2075,7 +2085,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A36" s="14" t="s">
         <v>156</v>
       </c>
@@ -2116,6 +2126,7 @@
     <mergeCell ref="H2:I2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2123,36 +2134,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{660B36E2-614D-4BFC-9DFD-65D5E3ED2816}">
   <dimension ref="A2:K34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="94" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView zoomScale="94" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="43.36328125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.453125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="15.40625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="43.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.46484375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="15.3984375" style="3" customWidth="1"/>
     <col min="4" max="4" width="0.86328125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="11.453125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="15.40625" style="3" customWidth="1"/>
-    <col min="7" max="16384" width="8.7265625" style="3"/>
+    <col min="5" max="5" width="11.46484375" style="3" customWidth="1"/>
+    <col min="6" max="6" width="15.3984375" style="3" customWidth="1"/>
+    <col min="7" max="16384" width="8.73046875" style="3"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" s="1"/>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="22" t="s">
         <v>159</v>
       </c>
-      <c r="C2" s="17"/>
+      <c r="C2" s="22"/>
       <c r="D2" s="2"/>
-      <c r="E2" s="17" t="s">
+      <c r="E2" s="22" t="s">
         <v>158</v>
       </c>
-      <c r="F2" s="17" t="s">
+      <c r="F2" s="22" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="15" t="s">
         <v>155</v>
       </c>
@@ -2163,212 +2174,212 @@
         <v>4</v>
       </c>
       <c r="D3" s="6"/>
-      <c r="E3" s="20" t="s">
+      <c r="E3" s="16" t="s">
         <v>160</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="17" t="s">
         <v>164</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="C4" s="18" t="s">
         <v>165</v>
       </c>
       <c r="D4" s="7"/>
-      <c r="E4" s="21" t="s">
+      <c r="E4" s="17" t="s">
         <v>162</v>
       </c>
-      <c r="F4" s="22" t="s">
+      <c r="F4" s="18" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.75">
-      <c r="A5" s="19" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A5" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="19" t="s">
+      <c r="C5" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19" t="s">
+      <c r="D5" s="24"/>
+      <c r="E5" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="19" t="s">
+      <c r="F5" s="24" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="23" t="s">
+      <c r="B6" s="19" t="s">
         <v>168</v>
       </c>
-      <c r="C6" s="23" t="s">
+      <c r="C6" s="19" t="s">
         <v>169</v>
       </c>
       <c r="D6" s="7"/>
-      <c r="E6" s="23" t="s">
+      <c r="E6" s="19" t="s">
         <v>166</v>
       </c>
-      <c r="F6" s="23" t="s">
+      <c r="F6" s="19" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="B7" s="23" t="s">
+      <c r="B7" s="19" t="s">
         <v>172</v>
       </c>
-      <c r="C7" s="23" t="s">
+      <c r="C7" s="19" t="s">
         <v>173</v>
       </c>
       <c r="D7" s="7"/>
-      <c r="E7" s="23" t="s">
+      <c r="E7" s="19" t="s">
         <v>170</v>
       </c>
-      <c r="F7" s="23" t="s">
+      <c r="F7" s="19" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="24" t="s">
+      <c r="B8" s="20" t="s">
         <v>176</v>
       </c>
-      <c r="C8" s="23" t="s">
+      <c r="C8" s="19" t="s">
         <v>177</v>
       </c>
       <c r="D8" s="7"/>
-      <c r="E8" s="23" t="s">
+      <c r="E8" s="19" t="s">
         <v>174</v>
       </c>
-      <c r="F8" s="23" t="s">
+      <c r="F8" s="19" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="B9" s="23" t="s">
+      <c r="B9" s="19" t="s">
         <v>179</v>
       </c>
-      <c r="C9" s="23" t="s">
+      <c r="C9" s="19" t="s">
         <v>180</v>
       </c>
       <c r="D9" s="7"/>
-      <c r="E9" s="23" t="s">
+      <c r="E9" s="19" t="s">
         <v>174</v>
       </c>
-      <c r="F9" s="23" t="s">
+      <c r="F9" s="19" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="24" t="s">
+      <c r="B10" s="20" t="s">
         <v>183</v>
       </c>
-      <c r="C10" s="23" t="s">
+      <c r="C10" s="19" t="s">
         <v>184</v>
       </c>
       <c r="D10" s="7"/>
-      <c r="E10" s="23" t="s">
+      <c r="E10" s="19" t="s">
         <v>181</v>
       </c>
-      <c r="F10" s="23" t="s">
+      <c r="F10" s="19" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="B11" s="23" t="s">
+      <c r="B11" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="23" t="s">
+      <c r="C11" s="19" t="s">
         <v>187</v>
       </c>
       <c r="D11" s="7"/>
-      <c r="E11" s="24" t="s">
+      <c r="E11" s="20" t="s">
         <v>185</v>
       </c>
-      <c r="F11" s="23" t="s">
+      <c r="F11" s="19" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="23" t="s">
+      <c r="B12" s="19" t="s">
         <v>189</v>
       </c>
-      <c r="C12" s="23" t="s">
+      <c r="C12" s="19" t="s">
         <v>190</v>
       </c>
       <c r="D12" s="7"/>
-      <c r="E12" s="24" t="s">
+      <c r="E12" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="F12" s="23" t="s">
+      <c r="F12" s="19" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="23" t="s">
+      <c r="B13" s="19" t="s">
         <v>193</v>
       </c>
-      <c r="C13" s="23" t="s">
+      <c r="C13" s="19" t="s">
         <v>194</v>
       </c>
       <c r="D13" s="7"/>
-      <c r="E13" s="24" t="s">
+      <c r="E13" s="20" t="s">
         <v>191</v>
       </c>
-      <c r="F13" s="23" t="s">
+      <c r="F13" s="19" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="23" t="s">
+      <c r="B14" s="19" t="s">
         <v>193</v>
       </c>
-      <c r="C14" s="23" t="s">
+      <c r="C14" s="19" t="s">
         <v>196</v>
       </c>
       <c r="D14" s="7"/>
-      <c r="E14" s="23" t="s">
+      <c r="E14" s="19" t="s">
         <v>174</v>
       </c>
-      <c r="F14" s="23" t="s">
+      <c r="F14" s="19" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15" s="8" t="s">
         <v>35</v>
       </c>
@@ -2378,133 +2389,133 @@
       <c r="E15" s="4"/>
       <c r="F15" s="7"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.75">
-      <c r="A16" s="19" t="s">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A16" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="B16" s="19" t="s">
+      <c r="B16" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="C16" s="19" t="s">
+      <c r="C16" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="D16" s="19"/>
-      <c r="E16" s="19" t="s">
+      <c r="D16" s="24"/>
+      <c r="E16" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="F16" s="19" t="s">
+      <c r="F16" s="24" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A17" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="B17" s="23" t="s">
+      <c r="B17" s="19" t="s">
         <v>199</v>
       </c>
-      <c r="C17" s="23" t="s">
+      <c r="C17" s="19" t="s">
         <v>200</v>
       </c>
       <c r="D17" s="7"/>
-      <c r="E17" s="23" t="s">
+      <c r="E17" s="19" t="s">
         <v>197</v>
       </c>
-      <c r="F17" s="23" t="s">
+      <c r="F17" s="19" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A18" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="B18" s="23" t="s">
+      <c r="B18" s="19" t="s">
         <v>202</v>
       </c>
-      <c r="C18" s="23" t="s">
+      <c r="C18" s="19" t="s">
         <v>203</v>
       </c>
       <c r="D18" s="7"/>
-      <c r="E18" s="23" t="s">
+      <c r="E18" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="F18" s="23" t="s">
+      <c r="F18" s="19" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A19" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="B19" s="24" t="s">
+      <c r="B19" s="20" t="s">
         <v>206</v>
       </c>
-      <c r="C19" s="23" t="s">
+      <c r="C19" s="19" t="s">
         <v>207</v>
       </c>
       <c r="D19" s="7"/>
-      <c r="E19" s="23" t="s">
+      <c r="E19" s="19" t="s">
         <v>204</v>
       </c>
-      <c r="F19" s="23" t="s">
+      <c r="F19" s="19" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A20" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="B20" s="23" t="s">
+      <c r="B20" s="19" t="s">
         <v>210</v>
       </c>
-      <c r="C20" s="23" t="s">
+      <c r="C20" s="19" t="s">
         <v>211</v>
       </c>
       <c r="D20" s="7"/>
-      <c r="E20" s="23" t="s">
+      <c r="E20" s="19" t="s">
         <v>208</v>
       </c>
-      <c r="F20" s="23" t="s">
+      <c r="F20" s="19" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A21" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="B21" s="23" t="s">
+      <c r="B21" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="C21" s="23" t="s">
+      <c r="C21" s="19" t="s">
         <v>213</v>
       </c>
       <c r="D21" s="7"/>
-      <c r="E21" s="23" t="s">
+      <c r="E21" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="F21" s="23" t="s">
+      <c r="F21" s="19" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A22" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="B22" s="24" t="s">
+      <c r="B22" s="20" t="s">
         <v>216</v>
       </c>
-      <c r="C22" s="23" t="s">
+      <c r="C22" s="19" t="s">
         <v>217</v>
       </c>
       <c r="D22" s="7"/>
-      <c r="E22" s="23" t="s">
+      <c r="E22" s="19" t="s">
         <v>214</v>
       </c>
-      <c r="F22" s="23" t="s">
+      <c r="F22" s="19" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A23" s="8" t="s">
         <v>48</v>
       </c>
@@ -2514,28 +2525,28 @@
       <c r="E23" s="7"/>
       <c r="F23" s="7"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B24" s="7"/>
       <c r="C24" s="7"/>
       <c r="D24" s="7"/>
       <c r="E24" s="7"/>
       <c r="F24" s="7"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A25" s="1"/>
-      <c r="B25" s="17" t="s">
+      <c r="B25" s="22" t="s">
         <v>159</v>
       </c>
-      <c r="C25" s="17"/>
+      <c r="C25" s="22"/>
       <c r="D25" s="2"/>
-      <c r="E25" s="17" t="s">
+      <c r="E25" s="22" t="s">
         <v>158</v>
       </c>
-      <c r="F25" s="17" t="s">
+      <c r="F25" s="22" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="16.5" x14ac:dyDescent="0.75">
+    <row r="26" spans="1:11" ht="15.75" x14ac:dyDescent="0.45">
       <c r="A26" s="11" t="s">
         <v>60</v>
       </c>
@@ -2553,147 +2564,147 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A27" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B27" s="23" t="s">
+      <c r="B27" s="19" t="s">
         <v>220</v>
       </c>
-      <c r="C27" s="23" t="s">
+      <c r="C27" s="19" t="s">
         <v>221</v>
       </c>
       <c r="D27" s="7"/>
-      <c r="E27" s="23" t="s">
+      <c r="E27" s="19" t="s">
         <v>218</v>
       </c>
-      <c r="F27" s="23" t="s">
+      <c r="F27" s="19" t="s">
         <v>219</v>
       </c>
-      <c r="J27" s="23"/>
-      <c r="K27" s="23"/>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="J27" s="19"/>
+      <c r="K27" s="19"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A28" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B28" s="23" t="s">
+      <c r="B28" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="C28" s="23" t="s">
+      <c r="C28" s="19" t="s">
         <v>223</v>
       </c>
       <c r="D28" s="7"/>
-      <c r="E28" s="23" t="s">
+      <c r="E28" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="F28" s="23" t="s">
+      <c r="F28" s="19" t="s">
         <v>222</v>
       </c>
-      <c r="J28" s="23"/>
-      <c r="K28" s="23"/>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="J28" s="19"/>
+      <c r="K28" s="19"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A29" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="B29" s="23" t="s">
+      <c r="B29" s="19" t="s">
         <v>225</v>
       </c>
-      <c r="C29" s="23" t="s">
+      <c r="C29" s="19" t="s">
         <v>226</v>
       </c>
       <c r="D29" s="7"/>
-      <c r="E29" s="23" t="s">
+      <c r="E29" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="F29" s="23" t="s">
+      <c r="F29" s="19" t="s">
         <v>224</v>
       </c>
-      <c r="J29" s="23"/>
-      <c r="K29" s="23"/>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="J29" s="19"/>
+      <c r="K29" s="19"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A30" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="23" t="s">
+      <c r="B30" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="C30" s="23" t="s">
+      <c r="C30" s="19" t="s">
         <v>228</v>
       </c>
       <c r="D30" s="7"/>
-      <c r="E30" s="23" t="s">
+      <c r="E30" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="F30" s="23" t="s">
+      <c r="F30" s="19" t="s">
         <v>227</v>
       </c>
-      <c r="J30" s="23"/>
-      <c r="K30" s="23"/>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="J30" s="19"/>
+      <c r="K30" s="19"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A31" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="B31" s="23" t="s">
+      <c r="B31" s="19" t="s">
         <v>230</v>
       </c>
-      <c r="C31" s="23" t="s">
+      <c r="C31" s="19" t="s">
         <v>231</v>
       </c>
       <c r="D31" s="7"/>
-      <c r="E31" s="23" t="s">
+      <c r="E31" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="F31" s="23" t="s">
+      <c r="F31" s="19" t="s">
         <v>229</v>
       </c>
-      <c r="J31" s="23"/>
-      <c r="K31" s="23"/>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="J31" s="19"/>
+      <c r="K31" s="19"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A32" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B32" s="23" t="s">
+      <c r="B32" s="19" t="s">
         <v>233</v>
       </c>
-      <c r="C32" s="23" t="s">
+      <c r="C32" s="19" t="s">
         <v>234</v>
       </c>
       <c r="D32" s="7"/>
-      <c r="E32" s="23" t="s">
+      <c r="E32" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="F32" s="23" t="s">
+      <c r="F32" s="19" t="s">
         <v>232</v>
       </c>
-      <c r="J32" s="23"/>
-      <c r="K32" s="23"/>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="J32" s="19"/>
+      <c r="K32" s="19"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A33" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="B33" s="23" t="s">
+      <c r="B33" s="19" t="s">
         <v>236</v>
       </c>
-      <c r="C33" s="23" t="s">
+      <c r="C33" s="19" t="s">
         <v>237</v>
       </c>
       <c r="D33" s="7"/>
-      <c r="E33" s="23" t="s">
+      <c r="E33" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="F33" s="23" t="s">
+      <c r="F33" s="19" t="s">
         <v>235</v>
       </c>
-      <c r="J33" s="23"/>
-      <c r="K33" s="23"/>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="J33" s="19"/>
+      <c r="K33" s="19"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A34" s="14" t="s">
         <v>156</v>
       </c>

</xml_diff>